<commit_message>
Added more interactivity; removed irrelevant cells; fixed some bugs
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -28,16 +28,16 @@
     <t>RMSE relative Error</t>
   </si>
   <si>
-    <t>Run1</t>
-  </si>
-  <si>
-    <t>Run2</t>
-  </si>
-  <si>
-    <t>Run3</t>
-  </si>
-  <si>
-    <t>Run4</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
   <si>
     <t>71-100</t>

</xml_diff>

<commit_message>
Added files for pyplis velocity analysis for Arve
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Run</t>
   </si>
@@ -74,15 +74,6 @@
   </si>
   <si>
     <t>RESTOA_ERBE</t>
-  </si>
-  <si>
-    <t>Top model net flux</t>
-  </si>
-  <si>
-    <t>SRF net flux</t>
-  </si>
-  <si>
-    <t>TOA  net flux</t>
   </si>
 </sst>
 </file>
@@ -551,9 +542,7 @@
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5">
         <v>-0.489</v>
       </c>
@@ -577,9 +566,7 @@
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6">
         <v>-0.489</v>
       </c>
@@ -603,9 +590,7 @@
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="C7">
         <v>0.537</v>
       </c>
@@ -647,9 +632,7 @@
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="C8">
         <v>1.47</v>
       </c>

</xml_diff>